<commit_message>
Finalized BOM and PCB
</commit_message>
<xml_diff>
--- a/Altium_Linda_SRAD_Avionics/Bill of Materials-Linda_SRAD_Avionics_V02.xlsx
+++ b/Altium_Linda_SRAD_Avionics/Bill of Materials-Linda_SRAD_Avionics_V02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0857040a5fc6d13c/Desktop/Altium_Projects/Linda-Avionics-Hardware/Altium_Linda_SRAD_Avionics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="8_{79BD77D4-8251-4D09-938F-EC45512BDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2949159A-5854-48AF-B538-6F6303EA8ACB}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="8_{79BD77D4-8251-4D09-938F-EC45512BDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C419A8-A269-4B44-BBE8-FE8330AF0E74}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2118,8 +2118,8 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F33" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2286,11 +2286,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>44994</v>
+        <v>44995</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>44994.009310995367</v>
+        <v>44995.725291782408</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -2833,10 +2833,10 @@
         <v>5</v>
       </c>
       <c r="M20" s="81">
-        <v>4</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="N20" s="81">
-        <v>20</v>
+        <v>50.18</v>
       </c>
       <c r="O20" s="65" t="s">
         <v>40</v>
@@ -3690,7 +3690,7 @@
       <c r="M39" s="45"/>
       <c r="N39" s="45">
         <f>SUM(N10:N38)</f>
-        <v>597.1</v>
+        <v>627.28000000000009</v>
       </c>
       <c r="O39" s="67"/>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="L41" s="101">
         <f>N39</f>
-        <v>597.1</v>
+        <v>627.28000000000009</v>
       </c>
       <c r="M41" s="102"/>
       <c r="N41" s="89" t="s">
@@ -3753,7 +3753,7 @@
       <c r="K42" s="6"/>
       <c r="L42" s="103">
         <f>L41/H41</f>
-        <v>119.42</v>
+        <v>125.45600000000002</v>
       </c>
       <c r="M42" s="103"/>
       <c r="N42" s="90" t="s">
@@ -3796,7 +3796,7 @@
       </c>
       <c r="K46" s="96">
         <f>L42-M10-M12-M13-M14-M15-M16-M19-M18-M17</f>
-        <v>67.670000000000016</v>
+        <v>73.706000000000031</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>195</v>
@@ -3817,7 +3817,7 @@
       <c r="K50" s="97"/>
       <c r="N50" s="98">
         <f>SUM(N10,N20,N22:N30,N32,N33,N34,N35,N36)</f>
-        <v>105.54</v>
+        <v>135.72000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>